<commit_message>
QUMO = Quercus montana
</commit_message>
<xml_diff>
--- a/Data/tree_rings/TRW_coord2.xlsx
+++ b/Data/tree_rings/TRW_coord2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\world\Documents\GitHub\growth_phenology\Data\tree_rings\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/EcoClimLab/growth_phenology/Data/tree_rings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE796778-F58F-4F08-9718-81058C63103E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9C1E91-50D5-5446-961D-9BDC14AFFF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRW_coord" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="436">
   <si>
     <t>Latitude</t>
   </si>
@@ -321,9 +321,6 @@
     <t>Quercus macrocarpa</t>
   </si>
   <si>
-    <t>Quercus mongolica</t>
-  </si>
-  <si>
     <t>Quercus rubra</t>
   </si>
   <si>
@@ -484,9 +481,6 @@
   </si>
   <si>
     <t>Bur oak</t>
-  </si>
-  <si>
-    <t>Mongolian oak</t>
   </si>
   <si>
     <t>Chestnut oak</t>
@@ -1787,21 +1781,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.7265625" style="7"/>
-    <col min="3" max="3" width="31.7265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="40.7265625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="17.7265625" style="7"/>
-    <col min="8" max="16384" width="17.7265625" style="6"/>
+    <col min="1" max="2" width="17.6640625" style="7"/>
+    <col min="3" max="3" width="31.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="17.6640625" style="7"/>
+    <col min="8" max="16384" width="17.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1812,7 +1806,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>2</v>
@@ -1824,7 +1818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>42.701533333333337</v>
       </c>
@@ -1832,10 +1826,10 @@
         <v>-73.839083333333335</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>11</v>
@@ -1847,7 +1841,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>41.569283300000002</v>
       </c>
@@ -1855,16 +1849,16 @@
         <v>-71.284033300000004</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>42.271616666666667</v>
       </c>
@@ -1872,10 +1866,10 @@
         <v>-76.626766666666654</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>12</v>
@@ -1887,7 +1881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>38.984566666666666</v>
       </c>
@@ -1895,10 +1889,10 @@
         <v>-77.242316666666667</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>42</v>
@@ -1910,7 +1904,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>38.989266666666666</v>
       </c>
@@ -1918,10 +1912,10 @@
         <v>-77.245800000000003</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>13</v>
@@ -1933,7 +1927,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>41.283000000000001</v>
       </c>
@@ -1941,10 +1935,10 @@
         <v>-74.233000000000004</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>15</v>
@@ -1956,7 +1950,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>41.283000000000001</v>
       </c>
@@ -1964,10 +1958,10 @@
         <v>-74.233000000000004</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>38</v>
@@ -1979,7 +1973,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>35.5</v>
       </c>
@@ -1987,10 +1981,10 @@
         <v>-82.6</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>16</v>
@@ -2002,7 +1996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>34.475662999999997</v>
       </c>
@@ -2010,16 +2004,16 @@
         <v>-84.329250999999999</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>41.381244000000002</v>
       </c>
@@ -2027,16 +2021,16 @@
         <v>-74.058852999999999</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>41.383000000000003</v>
       </c>
@@ -2044,10 +2038,10 @@
         <v>-74.016999999999996</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>12</v>
@@ -2059,7 +2053,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>41.383000000000003</v>
       </c>
@@ -2067,10 +2061,10 @@
         <v>-74.016999999999996</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
@@ -2082,7 +2076,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>36.875186999999997</v>
       </c>
@@ -2090,16 +2084,16 @@
         <v>-83.360369000000006</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>36.875186999999997</v>
       </c>
@@ -2107,16 +2101,16 @@
         <v>-83.360369000000006</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>36.875186999999997</v>
       </c>
@@ -2124,16 +2118,16 @@
         <v>-83.360369000000006</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>37.536433333333335</v>
       </c>
@@ -2141,10 +2135,10 @@
         <v>-79.494883333333334</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>16</v>
@@ -2156,7 +2150,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>40.875455600000002</v>
       </c>
@@ -2164,10 +2158,10 @@
         <v>-73.790033300000005</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>13</v>
@@ -2179,7 +2173,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>32.772449999999999</v>
       </c>
@@ -2187,10 +2181,10 @@
         <v>-84.906533333333343</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>17</v>
@@ -2202,7 +2196,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>38.65</v>
       </c>
@@ -2210,16 +2204,16 @@
         <v>-79.366699999999994</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>43.288583333333328</v>
       </c>
@@ -2227,10 +2221,10 @@
         <v>-76.388533333333342</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>12</v>
@@ -2242,7 +2236,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>37.153092999999998</v>
       </c>
@@ -2250,16 +2244,16 @@
         <v>-84.269876999999994</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>37.130000000000003</v>
       </c>
@@ -2267,16 +2261,16 @@
         <v>-84.27</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>37.130000000000003</v>
       </c>
@@ -2284,16 +2278,16 @@
         <v>-84.27</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>37.130000000000003</v>
       </c>
@@ -2301,16 +2295,16 @@
         <v>-84.27</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>35.742866666666664</v>
       </c>
@@ -2321,7 +2315,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>15</v>
@@ -2333,7 +2327,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>37.769433333333332</v>
       </c>
@@ -2341,10 +2335,10 @@
         <v>-79.241516666666669</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>12</v>
@@ -2356,7 +2350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>37.770716666666665</v>
       </c>
@@ -2364,10 +2358,10 @@
         <v>-79.241600000000005</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>44</v>
@@ -2379,7 +2373,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>37.769433333333332</v>
       </c>
@@ -2387,10 +2381,10 @@
         <v>-79.241516666666669</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>18</v>
@@ -2402,7 +2396,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>37.768683333333335</v>
       </c>
@@ -2410,10 +2404,10 @@
         <v>-79.242383333333336</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>20</v>
@@ -2425,7 +2419,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>31.021277999999999</v>
       </c>
@@ -2433,33 +2427,33 @@
         <v>-87.248272999999998</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B32" s="7">
         <v>-83.835749000000007</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>34.76</v>
       </c>
@@ -2467,16 +2461,16 @@
         <v>-84.3</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>34.76</v>
       </c>
@@ -2484,16 +2478,16 @@
         <v>-84.3</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>44.116700999999999</v>
       </c>
@@ -2501,16 +2495,16 @@
         <v>-73.810458999999994</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>43.354366666666671</v>
       </c>
@@ -2518,10 +2512,10 @@
         <v>-73.690266666666673</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>11</v>
@@ -2533,7 +2527,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>43.907716700000002</v>
       </c>
@@ -2541,16 +2535,16 @@
         <v>-74.218033300000002</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>43.069875000000003</v>
       </c>
@@ -2558,16 +2552,16 @@
         <v>-73.286652000000004</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>43.069875000000003</v>
       </c>
@@ -2575,16 +2569,16 @@
         <v>-73.286652000000004</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>43.069875000000003</v>
       </c>
@@ -2592,16 +2586,16 @@
         <v>-73.286652000000004</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>43.068333333333335</v>
       </c>
@@ -2609,10 +2603,10 @@
         <v>-73.289999999999992</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>12</v>
@@ -2624,7 +2618,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>43.068333333333335</v>
       </c>
@@ -2632,10 +2626,10 @@
         <v>-73.289999999999992</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>16</v>
@@ -2647,7 +2641,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>43.062666666666665</v>
       </c>
@@ -2655,10 +2649,10 @@
         <v>-73.29816666666666</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>17</v>
@@ -2670,7 +2664,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>39.6569</v>
       </c>
@@ -2678,10 +2672,10 @@
         <v>-78.400533333333343</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>44</v>
@@ -2693,7 +2687,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>40.921599999999998</v>
       </c>
@@ -2701,10 +2695,10 @@
         <v>-73.929700000000011</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>18</v>
@@ -2716,7 +2710,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>43.684399999999997</v>
       </c>
@@ -2724,10 +2718,10 @@
         <v>-73.602466666666658</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
@@ -2739,7 +2733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>42.53</v>
       </c>
@@ -2747,16 +2741,16 @@
         <v>-72.180000000000007</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>42.53</v>
       </c>
@@ -2764,16 +2758,16 @@
         <v>-72.180000000000007</v>
       </c>
       <c r="C48" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>258</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>260</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>41.331633333333336</v>
       </c>
@@ -2781,10 +2775,10 @@
         <v>-74.657900000000012</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>38</v>
@@ -2796,7 +2790,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>41.331633333333336</v>
       </c>
@@ -2804,10 +2798,10 @@
         <v>-74.657900000000012</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>15</v>
@@ -2819,7 +2813,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>31.22</v>
       </c>
@@ -2827,16 +2821,16 @@
         <v>-84.47</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>37.675466666666665</v>
       </c>
@@ -2844,10 +2838,10 @@
         <v>-79.288033333333331</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>16</v>
@@ -2859,7 +2853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>37.674866666666667</v>
       </c>
@@ -2867,10 +2861,10 @@
         <v>-79.28413333333333</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>17</v>
@@ -2882,7 +2876,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>34.328800000000001</v>
       </c>
@@ -2890,16 +2884,16 @@
         <v>-85.246300000000005</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>43.174666666666667</v>
       </c>
@@ -2907,10 +2901,10 @@
         <v>-73.816833333333335</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>14</v>
@@ -2922,7 +2916,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>43.174666666666667</v>
       </c>
@@ -2930,16 +2924,16 @@
         <v>-73.816833333333335</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>42.794966666666667</v>
       </c>
@@ -2947,10 +2941,10 @@
         <v>-73.860050000000001</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>42</v>
@@ -2962,7 +2956,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>42.791466666666665</v>
       </c>
@@ -2970,10 +2964,10 @@
         <v>-73.858549999999994</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>16</v>
@@ -2985,7 +2979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>37.187032000000002</v>
       </c>
@@ -2993,16 +2987,16 @@
         <v>-86.103960999999998</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>41.041499999999999</v>
       </c>
@@ -3010,10 +3004,10 @@
         <v>-72.284533333333329</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>13</v>
@@ -3025,7 +3019,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>42.608583333333335</v>
       </c>
@@ -3033,10 +3027,10 @@
         <v>-74.318150000000003</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>17</v>
@@ -3048,7 +3042,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>42.060899999999997</v>
       </c>
@@ -3056,10 +3050,10 @@
         <v>-72.300899999999999</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>12</v>
@@ -3071,7 +3065,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>41.801199999999994</v>
       </c>
@@ -3079,10 +3073,10 @@
         <v>-74.105683333333332</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>42</v>
@@ -3094,7 +3088,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>41.798633333333335</v>
       </c>
@@ -3102,10 +3096,10 @@
         <v>-74.112549999999999</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>19</v>
@@ -3117,7 +3111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>41.809999999999995</v>
       </c>
@@ -3125,10 +3119,10 @@
         <v>-74.099049999999991</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>18</v>
@@ -3140,7 +3134,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>41.737966666666665</v>
       </c>
@@ -3148,10 +3142,10 @@
         <v>-74.20471666666667</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>11</v>
@@ -3163,7 +3157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>41.763800000000003</v>
       </c>
@@ -3171,10 +3165,10 @@
         <v>-74.124649999999988</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>17</v>
@@ -3186,7 +3180,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>41.789633333333335</v>
       </c>
@@ -3194,10 +3188,10 @@
         <v>-74.125616666666659</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>21</v>
@@ -3209,7 +3203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>42.542198999999997</v>
       </c>
@@ -3217,16 +3211,16 @@
         <v>-72.486699999999999</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>42.008800000000001</v>
       </c>
@@ -3234,10 +3228,10 @@
         <v>-73.918750000000003</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E70" s="7" t="s">
         <v>18</v>
@@ -3249,7 +3243,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>42.011366666666667</v>
       </c>
@@ -3257,10 +3251,10 @@
         <v>-73.920733333333345</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E71" s="7" t="s">
         <v>17</v>
@@ -3272,7 +3266,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>42.011366666666667</v>
       </c>
@@ -3280,10 +3274,10 @@
         <v>-73.920733333333345</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>12</v>
@@ -3295,7 +3289,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>43.228050000000003</v>
       </c>
@@ -3303,10 +3297,10 @@
         <v>-70.6892</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>17</v>
@@ -3318,7 +3312,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>37.735050000000001</v>
       </c>
@@ -3326,10 +3320,10 @@
         <v>-79.223966666666669</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E74" s="7" t="s">
         <v>42</v>
@@ -3341,7 +3335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>37.730766666666668</v>
       </c>
@@ -3349,10 +3343,10 @@
         <v>-79.223883333333333</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>21</v>
@@ -3364,7 +3358,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>39.262112999999999</v>
       </c>
@@ -3372,33 +3366,33 @@
         <v>-80.997377999999998</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E76" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B77" s="7">
         <v>-71.266750000000002</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E77" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
         <v>42.845140000000001</v>
       </c>
@@ -3406,16 +3400,16 @@
         <v>-72.447299999999998</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
         <v>42.845140000000001</v>
       </c>
@@ -3423,16 +3417,16 @@
         <v>-72.447299999999998</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
         <v>42.847709999999999</v>
       </c>
@@ -3440,16 +3434,16 @@
         <v>-72.447500000000005</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>42.844169999999998</v>
       </c>
@@ -3457,16 +3451,16 @@
         <v>-72.449759999999998</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>42.844169999999998</v>
       </c>
@@ -3474,16 +3468,16 @@
         <v>-72.449759999999998</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>42.844169999999998</v>
       </c>
@@ -3491,16 +3485,16 @@
         <v>-72.449759999999998</v>
       </c>
       <c r="C83" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D83" s="7" t="s">
         <v>264</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>266</v>
       </c>
       <c r="E83" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>42.844169999999998</v>
       </c>
@@ -3508,16 +3502,16 @@
         <v>-72.449759999999998</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E84" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>39.878466666666668</v>
       </c>
@@ -3525,10 +3519,10 @@
         <v>-76.386366666666675</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E85" s="7" t="s">
         <v>12</v>
@@ -3540,7 +3534,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>39.881033333333335</v>
       </c>
@@ -3548,10 +3542,10 @@
         <v>-76.390733333333344</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E86" s="7" t="s">
         <v>21</v>
@@ -3563,7 +3557,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>39.878466666666668</v>
       </c>
@@ -3571,10 +3565,10 @@
         <v>-76.386366666666675</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E87" s="7" t="s">
         <v>18</v>
@@ -3586,7 +3580,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>39.883333333333333</v>
       </c>
@@ -3594,10 +3588,10 @@
         <v>-76.389750000000006</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E88" s="7" t="s">
         <v>16</v>
@@ -3609,7 +3603,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
         <v>42.53</v>
       </c>
@@ -3617,16 +3611,16 @@
         <v>-72.180000000000007</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E89" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
         <v>41.710008000000002</v>
       </c>
@@ -3634,16 +3628,16 @@
         <v>-74.247273000000007</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>41.710008000000002</v>
       </c>
@@ -3651,16 +3645,16 @@
         <v>-74.247273000000007</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>41.705475</v>
       </c>
@@ -3668,16 +3662,16 @@
         <v>-74.248466699999994</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>41.705475</v>
       </c>
@@ -3685,16 +3679,16 @@
         <v>-74.251715000000004</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>41.705475</v>
       </c>
@@ -3702,16 +3696,16 @@
         <v>-74.251715000000004</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>43.2</v>
       </c>
@@ -3719,16 +3713,16 @@
         <v>-71.166700000000006</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
         <v>42.471333333333334</v>
       </c>
@@ -3736,10 +3730,10 @@
         <v>-74.925816666666677</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>12</v>
@@ -3751,7 +3745,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
         <v>42.831366000000003</v>
       </c>
@@ -3759,16 +3753,16 @@
         <v>-72.439199000000002</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
         <v>39.058116666666663</v>
       </c>
@@ -3776,10 +3770,10 @@
         <v>-77.329916666666662</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>17</v>
@@ -3791,7 +3785,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
         <v>43.418266666666668</v>
       </c>
@@ -3799,10 +3793,10 @@
         <v>-73.755083333333332</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>12</v>
@@ -3814,7 +3808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
         <v>43.421666666666667</v>
       </c>
@@ -3822,10 +3816,10 @@
         <v>-73.569999999999993</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E100" s="7" t="s">
         <v>44</v>
@@ -3837,7 +3831,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
         <v>43.417499999999997</v>
       </c>
@@ -3845,10 +3839,10 @@
         <v>-73.728999999999999</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>19</v>
@@ -3860,7 +3854,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
         <v>42.199420000000003</v>
       </c>
@@ -3868,16 +3862,16 @@
         <v>-73.864774999999995</v>
       </c>
       <c r="C102" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D102" s="7" t="s">
         <v>296</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
         <v>42.199420000000003</v>
       </c>
@@ -3885,16 +3879,16 @@
         <v>-73.864774999999995</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
         <v>43.806333333333328</v>
       </c>
@@ -3902,10 +3896,10 @@
         <v>-74.609549999999999</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>6</v>
@@ -3917,7 +3911,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
         <v>37.774234999999997</v>
       </c>
@@ -3925,16 +3919,16 @@
         <v>-83.661336000000006</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E105" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
         <v>39.729126000000001</v>
       </c>
@@ -3942,16 +3936,16 @@
         <v>-74.617548999999997</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E106" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
         <v>43.231380000000001</v>
       </c>
@@ -3959,16 +3953,16 @@
         <v>-74.522540000000006</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
         <v>41.376069999999999</v>
       </c>
@@ -3976,16 +3970,16 @@
         <v>-74.115521999999999</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
         <v>44.528399999999998</v>
       </c>
@@ -3993,16 +3987,16 @@
         <v>-71.638050000000007</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
         <v>43.057333333333332</v>
       </c>
@@ -4010,10 +4004,10 @@
         <v>-73.351833333333332</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>50</v>
@@ -4025,7 +4019,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
         <v>43.349633300000001</v>
       </c>
@@ -4033,16 +4027,16 @@
         <v>-78.661233300000006</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
         <v>34.357419</v>
       </c>
@@ -4050,16 +4044,16 @@
         <v>-87.427426999999994</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E112" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
         <v>34.357419</v>
       </c>
@@ -4067,16 +4061,16 @@
         <v>-87.427426999999994</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
         <v>32.850900000000003</v>
       </c>
@@ -4084,16 +4078,16 @@
         <v>-84.4803</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E114" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="7">
         <v>41.186</v>
       </c>
@@ -4101,10 +4095,10 @@
         <v>-74.268050000000002</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E115" s="7" t="s">
         <v>15</v>
@@ -4116,7 +4110,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
         <v>43.187999999999995</v>
       </c>
@@ -4124,10 +4118,10 @@
         <v>-73.498833333333337</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E116" s="7" t="s">
         <v>42</v>
@@ -4139,24 +4133,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B117" s="7">
         <v>-89.127605000000003</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
         <v>41.117066700000002</v>
       </c>
@@ -4167,13 +4161,13 @@
         <v>29</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E118" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
         <v>42.49</v>
       </c>
@@ -4181,16 +4175,16 @@
         <v>-71.88</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E119" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
         <v>42.682449999999996</v>
       </c>
@@ -4198,10 +4192,10 @@
         <v>-77.429966666666672</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E120" s="7" t="s">
         <v>12</v>
@@ -4213,7 +4207,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
         <v>43.119135</v>
       </c>
@@ -4221,16 +4215,16 @@
         <v>-76.386846000000006</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E121" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
         <v>44.555753000000003</v>
       </c>
@@ -4238,16 +4232,16 @@
         <v>-73.113145000000003</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E122" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
         <v>44.555753000000003</v>
       </c>
@@ -4255,16 +4249,16 @@
         <v>-73.113145000000003</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E123" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
         <v>44.555753000000003</v>
       </c>
@@ -4272,16 +4266,16 @@
         <v>-73.113145000000003</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
         <v>42.4230333</v>
       </c>
@@ -4289,16 +4283,16 @@
         <v>-78.894499999999994</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>40.824689999999997</v>
       </c>
@@ -4306,10 +4300,10 @@
         <v>-91.391817000000003</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>40.716610000000003</v>
       </c>
@@ -4317,10 +4311,10 @@
         <v>-91.981866999999994</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>41.908174000000002</v>
       </c>
@@ -4328,10 +4322,10 @@
         <v>-91.512773999999993</v>
       </c>
       <c r="C128" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>38.349770999999997</v>
       </c>
@@ -4339,10 +4333,10 @@
         <v>-87.828126999999995</v>
       </c>
       <c r="C129" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>37.529400000000003</v>
       </c>
@@ -4350,10 +4344,10 @@
         <v>-88.982799999999997</v>
       </c>
       <c r="C130" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>39.395555000000002</v>
       </c>
@@ -4361,10 +4355,10 @@
         <v>-88.161265</v>
       </c>
       <c r="C131" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>37.6</v>
       </c>
@@ -4372,10 +4366,10 @@
         <v>-89.2</v>
       </c>
       <c r="C132" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>40.138291000000002</v>
       </c>
@@ -4383,10 +4377,10 @@
         <v>-87.745765000000006</v>
       </c>
       <c r="C133" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>39.982858</v>
       </c>
@@ -4394,10 +4388,10 @@
         <v>-89.852411000000004</v>
       </c>
       <c r="C134" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>41.307161000000001</v>
       </c>
@@ -4405,10 +4399,10 @@
         <v>-88.993812000000005</v>
       </c>
       <c r="C135" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>41.664710999999997</v>
       </c>
@@ -4416,10 +4410,10 @@
         <v>-86.508244000000005</v>
       </c>
       <c r="C136" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="8">
         <v>39.060237000000001</v>
       </c>
@@ -4427,10 +4421,10 @@
         <v>-86.279252</v>
       </c>
       <c r="C137" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>41.126196999999998</v>
       </c>
@@ -4438,10 +4432,10 @@
         <v>-85.109915000000001</v>
       </c>
       <c r="C138" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>38.729999999999997</v>
       </c>
@@ -4449,10 +4443,10 @@
         <v>-86.42</v>
       </c>
       <c r="C139" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>41.518301000000001</v>
       </c>
@@ -4460,10 +4454,10 @@
         <v>-84.866101</v>
       </c>
       <c r="C140" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>40.348061999999999</v>
       </c>
@@ -4471,10 +4465,10 @@
         <v>-85.438847999999993</v>
       </c>
       <c r="C141" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>38.229087</v>
       </c>
@@ -4482,10 +4476,10 @@
         <v>-87.366518999999997</v>
       </c>
       <c r="C142" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>39.25</v>
       </c>
@@ -4493,10 +4487,10 @@
         <v>-86.89</v>
       </c>
       <c r="C143" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>39.158302999999997</v>
       </c>
@@ -4504,10 +4498,10 @@
         <v>-86.493393999999995</v>
       </c>
       <c r="C144" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>39.2361</v>
       </c>
@@ -4515,10 +4509,10 @@
         <v>-86.220399999999998</v>
       </c>
       <c r="C145" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>39.505057000000001</v>
       </c>
@@ -4526,10 +4520,10 @@
         <v>-85.669106999999997</v>
       </c>
       <c r="C146" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="9">
         <v>39.3232</v>
       </c>
@@ -4537,10 +4531,10 @@
         <v>-86.4131</v>
       </c>
       <c r="C147" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>41.339478999999997</v>
       </c>
@@ -4548,10 +4542,10 @@
         <v>-85.763454999999993</v>
       </c>
       <c r="C148" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>38.54</v>
       </c>
@@ -4559,10 +4553,10 @@
         <v>-86.45</v>
       </c>
       <c r="C149" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>38.370710000000003</v>
       </c>
@@ -4570,10 +4564,10 @@
         <v>-87.717270999999997</v>
       </c>
       <c r="C150" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>37.984732000000001</v>
       </c>
@@ -4581,10 +4575,10 @@
         <v>-87.512484999999998</v>
       </c>
       <c r="C151" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="9">
         <v>45.559800000000003</v>
       </c>
@@ -4592,10 +4586,10 @@
         <v>-84.713800000000006</v>
       </c>
       <c r="C152" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>41.827776</v>
       </c>
@@ -4603,10 +4597,10 @@
         <v>-86.623330999999993</v>
       </c>
       <c r="C153" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>38.620427999999997</v>
       </c>
@@ -4614,10 +4608,10 @@
         <v>-90.694719000000006</v>
       </c>
       <c r="C154" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="9">
         <v>38.744100000000003</v>
       </c>
@@ -4625,10 +4619,10 @@
         <v>-92.2</v>
       </c>
       <c r="C155" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>35.358468000000002</v>
       </c>
@@ -4636,10 +4630,10 @@
         <v>-83.930323000000001</v>
       </c>
       <c r="C156" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>35.031278</v>
       </c>
@@ -4647,10 +4641,10 @@
         <v>-83.257677999999999</v>
       </c>
       <c r="C157" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>35.598030000000001</v>
       </c>
@@ -4658,10 +4652,10 @@
         <v>-83.422387000000001</v>
       </c>
       <c r="C158" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>40.137555999999996</v>
       </c>
@@ -4669,10 +4663,10 @@
         <v>-83.907942000000006</v>
       </c>
       <c r="C159" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>41.553987999999997</v>
       </c>
@@ -4680,10 +4674,10 @@
         <v>-84.362049999999996</v>
       </c>
       <c r="C160" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>39.578251999999999</v>
       </c>
@@ -4691,10 +4685,10 @@
         <v>-84.738961000000003</v>
       </c>
       <c r="C161" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>40.880000000000003</v>
       </c>
@@ -4702,10 +4696,10 @@
         <v>-81.75</v>
       </c>
       <c r="C162" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>39.349398999999998</v>
       </c>
@@ -4713,10 +4707,10 @@
         <v>-82.072413999999995</v>
       </c>
       <c r="C163" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>40.69</v>
       </c>
@@ -4724,10 +4718,10 @@
         <v>-77.75</v>
       </c>
       <c r="C164" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>35.621211000000002</v>
       </c>
@@ -4735,10 +4729,10 @@
         <v>-83.086316999999994</v>
       </c>
       <c r="C165" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>35.553618</v>
       </c>
@@ -4746,10 +4740,10 @@
         <v>-83.838504</v>
       </c>
       <c r="C166" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>35.706690999999999</v>
       </c>
@@ -4757,10 +4751,10 @@
         <v>-83.33878</v>
       </c>
       <c r="C167" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>35.689200999999997</v>
       </c>
@@ -4768,10 +4762,10 @@
         <v>-83.611080000000001</v>
       </c>
       <c r="C168" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>35.677073</v>
       </c>
@@ -4779,10 +4773,10 @@
         <v>-83.397133999999994</v>
       </c>
       <c r="C169" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>35.664957000000001</v>
       </c>
@@ -4790,10 +4784,10 @@
         <v>-83.463175000000007</v>
       </c>
       <c r="C170" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>35.594862999999997</v>
       </c>
@@ -4801,7 +4795,7 @@
         <v>-83.916167000000002</v>
       </c>
       <c r="C171" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -4820,30 +4814,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7265625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="34.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>47</v>
       </c>
@@ -4851,10 +4845,10 @@
         <v>58</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -4862,10 +4856,10 @@
         <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -4873,10 +4867,10 @@
         <v>60</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
@@ -4884,10 +4878,10 @@
         <v>61</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -4895,10 +4889,10 @@
         <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -4906,10 +4900,10 @@
         <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -4917,10 +4911,10 @@
         <v>64</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -4928,21 +4922,21 @@
         <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -4950,21 +4944,21 @@
         <v>67</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -4972,10 +4966,10 @@
         <v>69</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -4983,10 +4977,10 @@
         <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -4994,10 +4988,10 @@
         <v>71</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -5005,10 +4999,10 @@
         <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
@@ -5016,10 +5010,10 @@
         <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
@@ -5027,10 +5021,10 @@
         <v>74</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -5038,10 +5032,10 @@
         <v>75</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -5049,10 +5043,10 @@
         <v>76</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -5060,10 +5054,10 @@
         <v>77</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -5071,10 +5065,10 @@
         <v>78</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
@@ -5082,10 +5076,10 @@
         <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -5093,10 +5087,10 @@
         <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
@@ -5104,10 +5098,10 @@
         <v>81</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
@@ -5115,10 +5109,10 @@
         <v>82</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
@@ -5126,10 +5120,10 @@
         <v>83</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
@@ -5137,10 +5131,10 @@
         <v>84</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
@@ -5148,10 +5142,10 @@
         <v>85</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
         <v>40</v>
       </c>
@@ -5159,10 +5153,10 @@
         <v>86</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
@@ -5170,10 +5164,10 @@
         <v>87</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
@@ -5181,10 +5175,10 @@
         <v>88</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
@@ -5192,10 +5186,10 @@
         <v>89</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -5203,10 +5197,10 @@
         <v>90</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
@@ -5214,10 +5208,10 @@
         <v>91</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>49</v>
       </c>
@@ -5225,21 +5219,21 @@
         <v>92</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
@@ -5247,10 +5241,10 @@
         <v>94</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>52</v>
       </c>
@@ -5258,10 +5252,10 @@
         <v>95</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>33</v>
       </c>
@@ -5269,10 +5263,10 @@
         <v>96</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -5280,155 +5274,155 @@
         <v>97</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -5441,12 +5435,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5673,15 +5664,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7C60C8E-4AD2-4631-AB8F-5A4A95076924}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C307AF-8C67-4B0B-9918-DE2565282750}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0929cee3-c006-4e24-b00c-75dc8ac246d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="87517bbe-da2b-4ee0-8afc-fdad99fef0aa"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5706,18 +5709,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C307AF-8C67-4B0B-9918-DE2565282750}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7C60C8E-4AD2-4631-AB8F-5A4A95076924}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0929cee3-c006-4e24-b00c-75dc8ac246d1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="87517bbe-da2b-4ee0-8afc-fdad99fef0aa"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>